<commit_message>
added mapping bean types..
</commit_message>
<xml_diff>
--- a/Domestic Standard Upload.xlsx
+++ b/Domestic Standard Upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\275261\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{413646EE-C9D4-4775-99E7-E422053F8816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA16A48A-9410-4241-B834-E67E207C7B0D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53CE06-312B-4614-8151-FA1A9D504034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="1" xr2:uid="{CE78BDE3-7438-4330-9B0A-3EEE37903C7F}"/>
   </bookViews>
@@ -22,9 +22,15 @@
     <definedName name="class">'Dmstc Stndrd Upld Tmplt'!$K$5</definedName>
     <definedName name="classx">'Dmstc Stndrd Upld Tmplt'!$K$5</definedName>
     <definedName name="color">'Dmstc Stndrd Upld Tmplt'!$E$5</definedName>
+    <definedName name="compretailer">'Dmstc Stndrd Upld Tmplt'!$N$5</definedName>
+    <definedName name="compretailprice">'Dmstc Stndrd Upld Tmplt'!$R$5</definedName>
+    <definedName name="currentcost">'Dmstc Stndrd Upld Tmplt'!$P$5</definedName>
     <definedName name="department">'Dmstc Stndrd Upld Tmplt'!$J$5</definedName>
     <definedName name="label">'Dmstc Stndrd Upld Tmplt'!$D$5</definedName>
     <definedName name="material">'Dmstc Stndrd Upld Tmplt'!$M$5</definedName>
+    <definedName name="omitcompretail">'Dmstc Stndrd Upld Tmplt'!$O$5</definedName>
+    <definedName name="orderonquantity">'Dmstc Stndrd Upld Tmplt'!$S$5</definedName>
+    <definedName name="originalcost">'Dmstc Stndrd Upld Tmplt'!$Q$5</definedName>
     <definedName name="ponumber">'Dmstc Stndrd Upld Tmplt'!$H$5</definedName>
     <definedName name="size">'Dmstc Stndrd Upld Tmplt'!$F$5</definedName>
     <definedName name="supplierid">'Dmstc Stndrd Upld Tmplt'!$I$5</definedName>
@@ -46,8 +52,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1145,7 +1149,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2017,26 +2021,26 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.5703125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="26" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="26" customWidth="1"/>
+    <col min="1" max="1" width="5.15625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="27.15625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.41796875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="14.83984375" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.41796875" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.15625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.41796875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="15.41796875" style="26" customWidth="1"/>
+    <col min="11" max="11" width="14.83984375" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.15">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.9" hidden="1">
+    <row r="2" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2106,7 +2110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="11" customFormat="1" ht="28.9">
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5">
         <v>5</v>
       </c>
@@ -2141,7 +2145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="94.5" hidden="1" customHeight="1">
+    <row r="4" spans="1:11" ht="94.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
         <v>6</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5">
         <v>7</v>
       </c>
@@ -2211,7 +2215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.9" hidden="1">
+    <row r="6" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5">
         <v>10</v>
       </c>
@@ -2246,7 +2250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
         <v>11</v>
       </c>
@@ -2281,7 +2285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.9" hidden="1">
+    <row r="8" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5">
         <v>13</v>
       </c>
@@ -2316,7 +2320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>15</v>
       </c>
@@ -2351,7 +2355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>16</v>
       </c>
@@ -2386,7 +2390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>17</v>
       </c>
@@ -2421,7 +2425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>18</v>
       </c>
@@ -2456,7 +2460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
         <v>19</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
         <v>20</v>
       </c>
@@ -2526,7 +2530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>21</v>
       </c>
@@ -2561,7 +2565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -2596,7 +2600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="16" customFormat="1" hidden="1">
+    <row r="17" spans="1:11" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>23</v>
       </c>
@@ -2629,7 +2633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>24</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>25</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>26</v>
       </c>
@@ -2734,7 +2738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>27</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>28</v>
       </c>
@@ -2804,7 +2808,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>29</v>
       </c>
@@ -2839,7 +2843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>30</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>31</v>
       </c>
@@ -2909,7 +2913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>32</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>33</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>34</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="28.9" hidden="1">
+    <row r="29" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>35</v>
       </c>
@@ -3047,7 +3051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>36</v>
       </c>
@@ -3082,7 +3086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>37</v>
       </c>
@@ -3117,7 +3121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="28.9" hidden="1">
+    <row r="32" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>38</v>
       </c>
@@ -3152,7 +3156,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5">
         <v>39</v>
       </c>
@@ -3187,7 +3191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5">
         <v>40</v>
       </c>
@@ -3222,7 +3226,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5">
         <v>41</v>
       </c>
@@ -3257,7 +3261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5">
         <v>42</v>
       </c>
@@ -3292,7 +3296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5">
         <v>43</v>
       </c>
@@ -3327,7 +3331,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="28.9" hidden="1">
+    <row r="38" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5">
         <v>45</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5">
         <v>46</v>
       </c>
@@ -3395,7 +3399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="28.9" hidden="1">
+    <row r="40" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="5">
         <v>47</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="28.9" hidden="1">
+    <row r="41" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5">
         <v>49</v>
       </c>
@@ -3465,7 +3469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="5">
         <v>50</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5">
         <v>51</v>
       </c>
@@ -3535,7 +3539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="43.15">
+    <row r="44" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5">
         <v>52</v>
       </c>
@@ -3570,7 +3574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="43.15" hidden="1">
+    <row r="45" spans="1:11" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5">
         <v>55</v>
       </c>
@@ -3605,7 +3609,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="28.9" hidden="1">
+    <row r="46" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5">
         <v>57</v>
       </c>
@@ -3640,7 +3644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="28.9" hidden="1">
+    <row r="47" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="5">
         <v>58</v>
       </c>
@@ -3675,7 +3679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="5">
         <v>61</v>
       </c>
@@ -3710,7 +3714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="28.9" hidden="1">
+    <row r="49" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5">
         <v>62</v>
       </c>
@@ -3743,7 +3747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="28.9" hidden="1">
+    <row r="50" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5">
         <v>63</v>
       </c>
@@ -3778,7 +3782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="28.9" hidden="1">
+    <row r="51" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="5">
         <v>66</v>
       </c>
@@ -3813,7 +3817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="5">
         <v>76</v>
       </c>
@@ -3848,7 +3852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="5">
         <v>77</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="5">
         <v>78</v>
       </c>
@@ -3914,7 +3918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="5">
         <v>83</v>
       </c>
@@ -3949,7 +3953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="5">
         <v>84</v>
       </c>
@@ -3984,7 +3988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="28.9" hidden="1">
+    <row r="57" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="5">
         <v>85</v>
       </c>
@@ -4019,7 +4023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="5">
         <v>90</v>
       </c>
@@ -4054,7 +4058,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="16" customFormat="1" hidden="1">
+    <row r="59" spans="1:11" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="5">
         <v>92</v>
       </c>
@@ -4089,7 +4093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="60" hidden="1" customHeight="1">
+    <row r="60" spans="1:11" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="5">
         <v>93</v>
       </c>
@@ -4124,7 +4128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="5">
         <v>98</v>
       </c>
@@ -4159,7 +4163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="5">
         <v>101</v>
       </c>
@@ -4194,7 +4198,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="5">
         <v>102</v>
       </c>
@@ -4229,7 +4233,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="43.15" hidden="1">
+    <row r="64" spans="1:11" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="5">
         <v>103</v>
       </c>
@@ -4264,7 +4268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="5">
         <v>104</v>
       </c>
@@ -4299,7 +4303,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="5">
         <v>105</v>
       </c>
@@ -4332,7 +4336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5">
         <v>106</v>
       </c>
@@ -4367,7 +4371,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="5">
         <v>116</v>
       </c>
@@ -4402,7 +4406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="5">
         <v>117</v>
       </c>
@@ -4437,7 +4441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="5">
         <v>118</v>
       </c>
@@ -4472,7 +4476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="5">
         <v>119</v>
       </c>
@@ -4507,7 +4511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="28.9" hidden="1">
+    <row r="72" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="5">
         <v>120</v>
       </c>
@@ -4542,7 +4546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="5">
         <v>121</v>
       </c>
@@ -4577,7 +4581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="5">
         <v>122</v>
       </c>
@@ -4612,7 +4616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5">
         <v>123</v>
       </c>
@@ -4647,7 +4651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="5">
         <v>125</v>
       </c>
@@ -4682,7 +4686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="5">
         <v>126</v>
       </c>
@@ -4717,7 +4721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="5">
         <v>129</v>
       </c>
@@ -4752,7 +4756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="5">
         <v>130</v>
       </c>
@@ -4787,7 +4791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="5">
         <v>131</v>
       </c>
@@ -4822,7 +4826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="28.9">
+    <row r="81" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="5">
         <v>132</v>
       </c>
@@ -4857,7 +4861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="5">
         <v>133</v>
       </c>
@@ -4892,7 +4896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="5">
         <v>138</v>
       </c>
@@ -4927,7 +4931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="5">
         <v>139</v>
       </c>
@@ -4962,7 +4966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="5">
         <v>141</v>
       </c>
@@ -4997,7 +5001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="5">
         <v>142</v>
       </c>
@@ -5032,7 +5036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="5">
         <v>147</v>
       </c>
@@ -5065,7 +5069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5">
         <v>148</v>
       </c>
@@ -5100,7 +5104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="5">
         <v>152</v>
       </c>
@@ -5133,7 +5137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="5">
         <v>153</v>
       </c>
@@ -5166,7 +5170,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="5">
         <v>154</v>
       </c>
@@ -5199,7 +5203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="28.9" hidden="1">
+    <row r="92" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="5">
         <v>155</v>
       </c>
@@ -5232,7 +5236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="24" customFormat="1" ht="28.9" hidden="1">
+    <row r="93" spans="1:11" s="24" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="5">
         <v>158</v>
       </c>
@@ -5267,7 +5271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="5">
         <v>164</v>
       </c>
@@ -5300,7 +5304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="5">
         <v>165</v>
       </c>
@@ -5333,7 +5337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="5">
         <v>167</v>
       </c>
@@ -5368,7 +5372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="5">
         <v>168</v>
       </c>
@@ -5403,7 +5407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="5">
         <v>170</v>
       </c>
@@ -5438,7 +5442,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="5">
         <v>173</v>
       </c>
@@ -5473,7 +5477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="5">
         <v>177</v>
       </c>
@@ -5508,7 +5512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="5">
         <v>178</v>
       </c>
@@ -5597,75 +5601,75 @@
   <dimension ref="A1:CV5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.7109375"/>
-    <col min="2" max="2" width="9.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.68359375"/>
+    <col min="2" max="2" width="9.41796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.41796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.41796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.41796875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="9.41796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.15625" style="39" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9" style="39" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="8.42578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="9.42578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="24" max="30" width="8.42578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.140625" style="39" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" style="39" customWidth="1"/>
+    <col min="13" max="18" width="8.41796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.41796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.15625" style="39" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9.41796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="24" max="30" width="8.41796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.15625" style="39" customWidth="1"/>
+    <col min="32" max="32" width="10.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.15625" style="39" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.68359375" style="39" customWidth="1"/>
     <col min="35" max="35" width="11" style="38" customWidth="1"/>
-    <col min="36" max="36" width="8.7109375" style="38"/>
-    <col min="37" max="38" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.68359375" style="38"/>
+    <col min="37" max="38" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11" style="38" customWidth="1"/>
-    <col min="40" max="44" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" style="38"/>
-    <col min="46" max="46" width="8.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="47" max="51" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.7109375" style="38"/>
-    <col min="53" max="55" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="40" max="44" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.68359375" style="38"/>
+    <col min="46" max="46" width="8.578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="47" max="51" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.68359375" style="38"/>
+    <col min="53" max="55" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="18" style="38" customWidth="1"/>
-    <col min="57" max="59" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="61" max="63" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.5703125" style="38" customWidth="1"/>
-    <col min="65" max="65" width="12.85546875" style="38" customWidth="1"/>
-    <col min="66" max="66" width="13.140625" style="38" customWidth="1"/>
-    <col min="67" max="67" width="11.85546875" style="38" customWidth="1"/>
-    <col min="68" max="68" width="15.85546875" style="38" customWidth="1"/>
-    <col min="69" max="69" width="13.140625" style="38" customWidth="1"/>
-    <col min="70" max="70" width="17.7109375" style="38" customWidth="1"/>
-    <col min="71" max="71" width="11.42578125" style="38" customWidth="1"/>
-    <col min="72" max="72" width="9.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="13.5703125" style="38" customWidth="1"/>
-    <col min="75" max="75" width="8.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="8.7109375" style="38"/>
-    <col min="78" max="80" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="82" max="83" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.140625" style="38" customWidth="1"/>
-    <col min="85" max="86" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="10.5703125" style="38" customWidth="1"/>
-    <col min="89" max="89" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="10.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="9.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="11.42578125" style="38" customWidth="1"/>
-    <col min="96" max="99" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="10.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="57" max="59" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="61" max="63" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.578125" style="38" customWidth="1"/>
+    <col min="65" max="65" width="12.83984375" style="38" customWidth="1"/>
+    <col min="66" max="66" width="13.15625" style="38" customWidth="1"/>
+    <col min="67" max="67" width="11.83984375" style="38" customWidth="1"/>
+    <col min="68" max="68" width="15.83984375" style="38" customWidth="1"/>
+    <col min="69" max="69" width="13.15625" style="38" customWidth="1"/>
+    <col min="70" max="70" width="17.68359375" style="38" customWidth="1"/>
+    <col min="71" max="71" width="11.41796875" style="38" customWidth="1"/>
+    <col min="72" max="72" width="9.41796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.578125" style="38" customWidth="1"/>
+    <col min="75" max="75" width="8.578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="8.68359375" style="38"/>
+    <col min="78" max="80" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="82" max="83" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.15625" style="38" customWidth="1"/>
+    <col min="85" max="86" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.578125" style="38" customWidth="1"/>
+    <col min="89" max="89" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="10.15625" style="38" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="9.41796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="11.41796875" style="38" customWidth="1"/>
+    <col min="96" max="99" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="10.15625" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="43.15">
+    <row r="1" spans="1:100" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
@@ -5967,7 +5971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:100" ht="14.65" thickBot="1">
+    <row r="2" spans="1:100" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -6269,7 +6273,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:100">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
       <c r="B3" s="52" t="s">
         <v>17</v>
@@ -6569,7 +6573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:100" s="29" customFormat="1" ht="57.95" thickBot="1">
+    <row r="4" spans="1:100" s="29" customFormat="1" ht="57.9" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="31" t="s">
         <v>248</v>
       </c>
@@ -6871,7 +6875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:100" hidden="1">
+    <row r="5" spans="1:100" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -6985,12 +6989,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7179,19 +7180,54 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9149A93E-C697-4066-B609-D79D6821B8AF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7799FA91-D05F-41CA-9D85-32D7401AB4F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ab086da4-aeaa-470f-88f5-e96437a646bb"/>
+    <ds:schemaRef ds:uri="cc44513a-9740-48a8-b9a6-11a9236a0f51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41DAFC0D-C589-4871-8EC2-037587728CED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41DAFC0D-C589-4871-8EC2-037587728CED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cc44513a-9740-48a8-b9a6-11a9236a0f51"/>
+    <ds:schemaRef ds:uri="ab086da4-aeaa-470f-88f5-e96437a646bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7799FA91-D05F-41CA-9D85-32D7401AB4F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9149A93E-C697-4066-B609-D79D6821B8AF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>